<commit_message>
Resolve isues related to PA-17 branch
</commit_message>
<xml_diff>
--- a/src/test/resources/test_files/input_file.xlsx
+++ b/src/test/resources/test_files/input_file.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nika.avalishvili/Desktop/Document/src/test/resources/test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{595346A8-06A3-104E-A97B-747AB2DCA79A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C482034-705C-2D41-8A02-CA8BA220E8E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="820" windowWidth="29140" windowHeight="17440" xr2:uid="{6BE14878-546C-9149-94ED-1CDA08022D16}"/>
   </bookViews>
@@ -413,7 +413,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="A2" sqref="A2:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -437,10 +437,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
-        <v>44886</v>
+        <v>44876</v>
       </c>
       <c r="B2" s="2">
-        <v>44804</v>
+        <v>44906</v>
       </c>
       <c r="C2" s="1">
         <v>3</v>
@@ -454,10 +454,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
-        <v>44887</v>
+        <v>44876</v>
       </c>
       <c r="B3" s="2">
-        <v>44834</v>
+        <v>44906</v>
       </c>
       <c r="C3" s="1">
         <v>12</v>
@@ -471,10 +471,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
-        <v>44886</v>
+        <v>44876</v>
       </c>
       <c r="B4" s="2">
-        <v>44804</v>
+        <v>44906</v>
       </c>
       <c r="C4" s="1">
         <v>4</v>
@@ -488,10 +488,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
-        <v>44887</v>
+        <v>44876</v>
       </c>
       <c r="B5" s="2">
-        <v>44834</v>
+        <v>44906</v>
       </c>
       <c r="C5" s="1">
         <v>5</v>

</xml_diff>

<commit_message>
Update implementation of sending id's with objects using MQ
</commit_message>
<xml_diff>
--- a/src/test/resources/test_files/input_file.xlsx
+++ b/src/test/resources/test_files/input_file.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nika.avalishvili/Desktop/Document/src/test/resources/test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C482034-705C-2D41-8A02-CA8BA220E8E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E06AC7D9-98C8-B84A-95C9-06CF454FD975}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="820" windowWidth="29140" windowHeight="17440" xr2:uid="{6BE14878-546C-9149-94ED-1CDA08022D16}"/>
   </bookViews>
@@ -413,7 +413,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E5"/>
+      <selection activeCell="A2" sqref="A2:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>